<commit_message>
Project Work Plan updated.
</commit_message>
<xml_diff>
--- a/documents/Project_Work_Plan.xlsx
+++ b/documents/Project_Work_Plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mxonu\Desktop\Projects\CENG407-408_TermProject\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mxonu\Desktop\Projects\CENG407-408_TermProject\PROJECT FILES\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B072CA-559E-417D-9CE8-8B2700EF81DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97A63DCF-0A55-41B7-9C5C-B177E3CFF262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -491,6 +491,27 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -511,27 +532,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -830,18 +830,18 @@
   <dimension ref="A1:T13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="U18" sqref="U18"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
       <c r="E1" s="6" t="s">
         <v>0</v>
       </c>
@@ -892,11 +892,11 @@
       </c>
     </row>
     <row r="2" spans="1:20" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
       <c r="D2" s="4" t="s">
         <v>29</v>
       </c>
@@ -950,11 +950,11 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
       <c r="D3" s="10" t="s">
         <v>16</v>
       </c>
@@ -976,11 +976,11 @@
       <c r="T3" s="2"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
       <c r="D4" s="10" t="s">
         <v>16</v>
       </c>
@@ -1002,11 +1002,11 @@
       <c r="T4" s="2"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
       <c r="D5" s="10" t="s">
         <v>16</v>
       </c>
@@ -1028,11 +1028,11 @@
       <c r="T5" s="2"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
       <c r="D6" s="10" t="s">
         <v>16</v>
       </c>
@@ -1054,11 +1054,11 @@
       <c r="T6" s="2"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
       <c r="D7" s="10" t="s">
         <v>16</v>
       </c>
@@ -1080,20 +1080,20 @@
       <c r="T7" s="2"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="9" t="s">
-        <v>22</v>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="31"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="22"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -1106,24 +1106,24 @@
       <c r="T8" s="2"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="11" t="s">
-        <v>24</v>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="9" t="s">
+        <v>22</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="21"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="27"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="28"/>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
@@ -1132,11 +1132,11 @@
       <c r="T9" s="2"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
       <c r="D10" s="11" t="s">
         <v>24</v>
       </c>
@@ -1149,8 +1149,8 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
-      <c r="N10" s="32"/>
-      <c r="O10" s="33"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="24"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
@@ -1158,11 +1158,11 @@
       <c r="T10" s="2"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
       <c r="D11" s="11" t="s">
         <v>24</v>
       </c>
@@ -1176,19 +1176,19 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
-      <c r="O11" s="22"/>
-      <c r="P11" s="23"/>
-      <c r="Q11" s="24"/>
+      <c r="O11" s="29"/>
+      <c r="P11" s="30"/>
+      <c r="Q11" s="31"/>
       <c r="R11" s="2"/>
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
       <c r="D12" s="11" t="s">
         <v>24</v>
       </c>
@@ -1204,17 +1204,17 @@
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
       <c r="P12" s="16"/>
-      <c r="Q12" s="25"/>
-      <c r="R12" s="25"/>
-      <c r="S12" s="25"/>
+      <c r="Q12" s="32"/>
+      <c r="R12" s="32"/>
+      <c r="S12" s="32"/>
       <c r="T12" s="2"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
       <c r="D13" s="11" t="s">
         <v>24</v>
       </c>
@@ -1237,14 +1237,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:C6"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="J9:N9"/>
     <mergeCell ref="O11:Q11"/>
@@ -1255,6 +1247,14 @@
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:C6"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
408 Project Work Plan updated.
</commit_message>
<xml_diff>
--- a/documents/Project_Work_Plan.xlsx
+++ b/documents/Project_Work_Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mxonu\Desktop\Projects\CENG407-408-TermProject\PROJECT FILES\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C25F11A4-D9B0-436C-9BB6-451413849AB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3EE0FA7-8FE7-4969-AC1B-A7667B9E8EAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -508,6 +508,52 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -517,40 +563,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -558,18 +570,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -875,12 +875,12 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
       <c r="E1" s="4" t="s">
         <v>0</v>
       </c>
@@ -931,11 +931,11 @@
       </c>
     </row>
     <row r="2" spans="1:20" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
       <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
@@ -989,18 +989,18 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
       <c r="D3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="30"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="32"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="36"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -1015,18 +1015,18 @@
       <c r="T3" s="1"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
       <c r="D4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="21"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="22"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="28"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -1041,20 +1041,20 @@
       <c r="T4" s="1"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="7" t="s">
-        <v>16</v>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="36"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="21"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -1067,12 +1067,12 @@
       <c r="T5" s="1"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="20" t="s">
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="15" t="s">
         <v>39</v>
       </c>
       <c r="E6" s="1"/>
@@ -1082,7 +1082,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
-      <c r="L6" s="29"/>
+      <c r="L6" s="19"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -1093,11 +1093,11 @@
       <c r="T6" s="1"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
       <c r="D7" s="7" t="s">
         <v>16</v>
       </c>
@@ -1119,12 +1119,12 @@
       <c r="T7" s="1"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="20" t="s">
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="15" t="s">
         <v>39</v>
       </c>
       <c r="E8" s="1"/>
@@ -1138,19 +1138,19 @@
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
-      <c r="P8" s="28"/>
+      <c r="P8" s="18"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="20" t="s">
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="15" t="s">
         <v>39</v>
       </c>
       <c r="E9" s="1"/>
@@ -1171,12 +1171,12 @@
       <c r="T9" s="1"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="20" t="s">
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="15" t="s">
         <v>39</v>
       </c>
       <c r="E10" s="1"/>
@@ -1197,12 +1197,12 @@
       <c r="T10" s="1"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="20" t="s">
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="15" t="s">
         <v>39</v>
       </c>
       <c r="E11" s="1"/>
@@ -1223,12 +1223,12 @@
       <c r="T11" s="1"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="20" t="s">
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="15" t="s">
         <v>39</v>
       </c>
       <c r="E12" s="1"/>
@@ -1244,17 +1244,17 @@
       <c r="O12" s="1"/>
       <c r="P12" s="9"/>
       <c r="Q12" s="9"/>
-      <c r="R12" s="26"/>
+      <c r="R12" s="16"/>
       <c r="S12" s="9"/>
       <c r="T12" s="1"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="20" t="s">
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="15" t="s">
         <v>39</v>
       </c>
       <c r="E13" s="1"/>
@@ -1270,17 +1270,17 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
-      <c r="R13" s="27"/>
+      <c r="R13" s="17"/>
       <c r="S13" s="10"/>
       <c r="T13" s="10"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="20" t="s">
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="15" t="s">
         <v>39</v>
       </c>
       <c r="E14" s="1"/>
@@ -1301,12 +1301,12 @@
       <c r="T14" s="10"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="20" t="s">
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="15" t="s">
         <v>39</v>
       </c>
       <c r="E15" s="1"/>
@@ -1323,11 +1323,17 @@
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="9"/>
-      <c r="S15" s="34"/>
-      <c r="T15" s="36"/>
+      <c r="S15" s="20"/>
+      <c r="T15" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A5:C5"/>
     <mergeCell ref="S15:T15"/>
     <mergeCell ref="A14:C14"/>
     <mergeCell ref="A15:C15"/>
@@ -1341,13 +1347,7 @@
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A5:C5"/>
     <mergeCell ref="A6:C6"/>
-    <mergeCell ref="E3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>